<commit_message>
improved pic, divider section corrections
</commit_message>
<xml_diff>
--- a/ltcc/ltccHV.xlsx
+++ b/ltcc/ltccHV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ungaro/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/opt/projects/clas12Nim/ltcc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C692A98B-AA55-3440-AF7B-0970B0445F67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28ABE66-9662-C144-96DC-20572850E776}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="1600" windowWidth="34740" windowHeight="26260" xr2:uid="{4968A2C1-2388-5A43-A3D6-87D4D1D74651}"/>
+    <workbookView xWindow="3660" yWindow="460" windowWidth="34740" windowHeight="23540" xr2:uid="{4968A2C1-2388-5A43-A3D6-87D4D1D74651}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,6 @@
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$37</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$37</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$2:$D$37</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$E$2:$E$37</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -182,10 +180,10 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="15"/>
+            <c:size val="20"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
@@ -195,6 +193,30 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="20"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-5DA4-174B-BB02-BAB487471936}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$37</c:f>
@@ -450,16 +472,14 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="15"/>
+            <c:symbol val="triangle"/>
+            <c:size val="25"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="tx2"/>
               </a:solidFill>
               <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -702,569 +722,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-913A-7445-8E38-93D1BF080365}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>AverageOld</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:srgbClr val="0070C0"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$2:$D$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1666.0833333333333</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1666.0833333333301</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-913A-7445-8E38-93D1BF080365}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$2:$E$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1292.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-913A-7445-8E38-93D1BF080365}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1322,7 +779,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1384,7 +841,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1417,10 +874,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.37463691137474964"/>
-          <c:y val="0.93505786853923012"/>
-          <c:w val="0.27132349959859547"/>
-          <c:h val="6.1850941352578223E-2"/>
+          <c:x val="0.27679963022129955"/>
+          <c:y val="0.61666528739548976"/>
+          <c:w val="0.44846047179221032"/>
+          <c:h val="0.19168092589662769"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1436,7 +893,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="4400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2392,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98FDEF0E-534A-F345-9D9F-D409BADA8452}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>